<commit_message>
fixed tan order incorrect calculation
</commit_message>
<xml_diff>
--- a/functionality dataframe test plan.xlsx
+++ b/functionality dataframe test plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://masseyhighschoolnz-my.sharepoint.com/personal/peddih9242_masseyhigh_school_nz/Documents/2022_Schoolwork/COM201/03_triangle_solver/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8826318C-DDB1-481F-97A8-3FB380211272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{8826318C-DDB1-481F-97A8-3FB380211272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{030C1B76-BB21-4E3D-B4E9-48036899B6D1}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{237C6F2B-1798-49C9-B44A-D1BB4CAF6C4C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Calculation Type</t>
   </si>
@@ -68,6 +68,27 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>36.87°</t>
+  </si>
+  <si>
+    <t>47°</t>
+  </si>
+  <si>
+    <t>3m</t>
+  </si>
+  <si>
+    <t>4m</t>
+  </si>
+  <si>
+    <t>5m</t>
+  </si>
+  <si>
+    <t>4mm</t>
+  </si>
+  <si>
+    <t>5mm</t>
   </si>
 </sst>
 </file>
@@ -422,7 +443,7 @@
   <dimension ref="A2:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,8 +478,8 @@
       <c r="D3">
         <v>5.36</v>
       </c>
-      <c r="E3">
-        <v>47</v>
+      <c r="E3" t="s">
+        <v>12</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -471,11 +492,11 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -483,28 +504,28 @@
       <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="G4">
-        <v>5</v>
+      <c r="G4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>36.869999999999997</v>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
       </c>
-      <c r="G5">
-        <v>36.869999999999997</v>
+      <c r="G5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed error when opp and adj given
</commit_message>
<xml_diff>
--- a/functionality dataframe test plan.xlsx
+++ b/functionality dataframe test plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://masseyhighschoolnz-my.sharepoint.com/personal/peddih9242_masseyhigh_school_nz/Documents/2022_Schoolwork/COM201/03_triangle_solver/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{8826318C-DDB1-481F-97A8-3FB380211272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{030C1B76-BB21-4E3D-B4E9-48036899B6D1}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="8_{8826318C-DDB1-481F-97A8-3FB380211272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D989F424-1E18-44BF-B043-2518A9DFC9DA}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{237C6F2B-1798-49C9-B44A-D1BB4CAF6C4C}"/>
   </bookViews>
@@ -35,60 +35,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
-  <si>
-    <t>Calculation Type</t>
-  </si>
-  <si>
-    <t>Trigonometry</t>
-  </si>
-  <si>
-    <t>Length 1</t>
-  </si>
-  <si>
-    <t>Length 2</t>
-  </si>
-  <si>
-    <t>Angle</t>
-  </si>
-  <si>
-    <t>Function</t>
-  </si>
-  <si>
-    <t>Answer</t>
-  </si>
-  <si>
-    <t>tan</t>
-  </si>
-  <si>
-    <t>Pythagoras</t>
-  </si>
-  <si>
-    <t>cos</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>36.87°</t>
-  </si>
-  <si>
-    <t>47°</t>
-  </si>
-  <si>
-    <t>3m</t>
-  </si>
-  <si>
-    <t>4m</t>
-  </si>
-  <si>
-    <t>5m</t>
-  </si>
-  <si>
-    <t>4mm</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>5mm</t>
+  </si>
+  <si>
+    <t>Calculation</t>
+  </si>
+  <si>
+    <t>Hypotenuse</t>
+  </si>
+  <si>
+    <t>Opposite</t>
+  </si>
+  <si>
+    <t>Adjacent</t>
+  </si>
+  <si>
+    <t>Angle 1</t>
+  </si>
+  <si>
+    <t>Angle 2</t>
+  </si>
+  <si>
+    <t>11.4km</t>
+  </si>
+  <si>
+    <t>9km</t>
+  </si>
+  <si>
+    <t>7km</t>
+  </si>
+  <si>
+    <t>3.41mm</t>
+  </si>
+  <si>
+    <t>3.66mm</t>
   </si>
 </sst>
 </file>
@@ -440,92 +422,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FAFADD2-3A8F-4A57-B4F0-4BF5FF794274}">
-  <dimension ref="A2:G5"/>
+  <dimension ref="A2:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
       <c r="E2" t="s">
         <v>4</v>
       </c>
       <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
       <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3">
-        <v>5.36</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
       </c>
       <c r="G3">
-        <v>5.36</v>
+        <v>36.869999999999997</v>
+      </c>
+      <c r="H3">
+        <v>53.13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="G4">
+        <v>47</v>
+      </c>
+      <c r="H4">
+        <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>52.13</v>
+      </c>
+      <c r="H5">
+        <v>37.869999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>